<commit_message>
moving model training to rubi
</commit_message>
<xml_diff>
--- a/culture_plate_counting/wasp_image_counting.xlsx
+++ b/culture_plate_counting/wasp_image_counting.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jmontgomery/OneDrive/Documents/IDbyDNA/Code/AbsoluteQuantification/culture_plate_counting/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC0F3C90-81C2-6146-AB85-57035E3F612B}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2140C56A-41B1-6642-86E5-881B56A0094E}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="920" yWindow="460" windowWidth="26040" windowHeight="14940" xr2:uid="{F88EBDB8-AFDE-DA4D-B2C5-563FAEF56804}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="26040" windowHeight="14940" xr2:uid="{F88EBDB8-AFDE-DA4D-B2C5-563FAEF56804}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="94">
   <si>
     <t>IDbyDNA-5383</t>
   </si>
@@ -294,21 +294,9 @@
     <t>15 confluent streaks</t>
   </si>
   <si>
-    <t>325 colonies</t>
-  </si>
-  <si>
-    <t>8 confluent colonies</t>
-  </si>
-  <si>
-    <t>425 colonies</t>
-  </si>
-  <si>
     <t>5 confluent streaks</t>
   </si>
   <si>
-    <t>103 colonies</t>
-  </si>
-  <si>
     <t>7 confluent streaks</t>
   </si>
   <si>
@@ -316,6 +304,15 @@
   </si>
   <si>
     <t>3 confluent streaks</t>
+  </si>
+  <si>
+    <t>9 confluent streaks</t>
+  </si>
+  <si>
+    <t>11 confluent streaks</t>
+  </si>
+  <si>
+    <t>17 confluent streaks</t>
   </si>
 </sst>
 </file>
@@ -673,10 +670,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DF95712E-7C7B-7042-B615-CB02932650F7}">
-  <dimension ref="A1:E81"/>
+  <dimension ref="A1:C81"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="E27" sqref="E27"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:C81"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -684,7 +681,7 @@
     <col min="1" max="1" width="13" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -692,193 +689,303 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>0</v>
       </c>
       <c r="B2" t="s">
         <v>3</v>
       </c>
-      <c r="D2">
-        <v>13.66</v>
-      </c>
-      <c r="E2">
-        <v>31.22</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="C2">
+        <f>14*100*1000</f>
+        <v>1400000</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>5</v>
       </c>
       <c r="B3" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="C3">
+        <f>22*100*1000</f>
+        <v>2200000</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>7</v>
       </c>
       <c r="B4" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="C4">
+        <f>4*100*1000</f>
+        <v>400000</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>8</v>
       </c>
       <c r="B5" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="C5">
+        <f>12*100*1000</f>
+        <v>1200000</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>9</v>
       </c>
       <c r="B6" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="C6">
+        <f>4*100*1000</f>
+        <v>400000</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>10</v>
       </c>
       <c r="B7" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="C7">
+        <f>12*100*1000</f>
+        <v>1200000</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>11</v>
       </c>
       <c r="B8" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="C8">
+        <f>15*100*1000</f>
+        <v>1500000</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>12</v>
       </c>
       <c r="B9" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="C9">
+        <f>15*100*1000</f>
+        <v>1500000</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>13</v>
       </c>
-      <c r="B10" t="s">
-        <v>87</v>
+      <c r="B10">
+        <v>325</v>
       </c>
       <c r="C10">
         <v>325000</v>
       </c>
-      <c r="D10">
-        <v>6.79</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>14</v>
       </c>
       <c r="B11" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+        <v>91</v>
+      </c>
+      <c r="C11">
+        <f>9*100*1000</f>
+        <v>900000</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>15</v>
       </c>
-      <c r="B12" t="s">
-        <v>89</v>
+      <c r="B12">
+        <v>425</v>
       </c>
       <c r="C12">
         <v>425000</v>
       </c>
-      <c r="D12">
-        <v>5.37</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>16</v>
       </c>
       <c r="B13" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+        <v>87</v>
+      </c>
+      <c r="C13">
+        <f>5*100*1000</f>
+        <v>500000</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>17</v>
       </c>
       <c r="B14" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+        <v>91</v>
+      </c>
+      <c r="C14">
+        <f>9*100*1000</f>
+        <v>900000</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>18</v>
       </c>
-      <c r="B15" t="s">
-        <v>91</v>
+      <c r="B15">
+        <v>105</v>
       </c>
       <c r="C15">
-        <v>103000</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+        <f>B15*1000</f>
+        <v>105000</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>19</v>
+      </c>
+      <c r="B16" t="s">
+        <v>92</v>
+      </c>
+      <c r="C16">
+        <f>11*100*1000</f>
+        <v>1100000</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>20</v>
       </c>
+      <c r="B17" t="s">
+        <v>88</v>
+      </c>
+      <c r="C17">
+        <f>7*100*1000</f>
+        <v>700000</v>
+      </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>21</v>
       </c>
+      <c r="B18">
+        <v>100</v>
+      </c>
+      <c r="C18">
+        <f>B18*1000</f>
+        <v>100000</v>
+      </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>22</v>
       </c>
+      <c r="B19" t="s">
+        <v>92</v>
+      </c>
+      <c r="C19">
+        <f>11*100*1000</f>
+        <v>1100000</v>
+      </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>23</v>
       </c>
+      <c r="B20" t="s">
+        <v>93</v>
+      </c>
+      <c r="C20">
+        <f>17*100*1000</f>
+        <v>1700000</v>
+      </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>24</v>
       </c>
+      <c r="B21" t="s">
+        <v>88</v>
+      </c>
+      <c r="C21">
+        <f>7*100*1000</f>
+        <v>700000</v>
+      </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>25</v>
       </c>
+      <c r="B22" t="s">
+        <v>87</v>
+      </c>
+      <c r="C22">
+        <f>5*100*1000</f>
+        <v>500000</v>
+      </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>26</v>
       </c>
+      <c r="B23" t="s">
+        <v>4</v>
+      </c>
+      <c r="C23">
+        <f>22*100*1000</f>
+        <v>2200000</v>
+      </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>27</v>
       </c>
+      <c r="B24" t="s">
+        <v>87</v>
+      </c>
+      <c r="C24">
+        <f>5*100*1000</f>
+        <v>500000</v>
+      </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>28</v>
       </c>
+      <c r="B25" t="s">
+        <v>90</v>
+      </c>
+      <c r="C25">
+        <f>3*100*1000</f>
+        <v>300000</v>
+      </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>29</v>
       </c>
+      <c r="B26" t="s">
+        <v>6</v>
+      </c>
+      <c r="C26">
+        <f>4*100*1000</f>
+        <v>400000</v>
+      </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
@@ -923,13 +1030,21 @@
       <c r="B30" t="s">
         <v>6</v>
       </c>
+      <c r="C30">
+        <f>4*100*1000</f>
+        <v>400000</v>
+      </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>34</v>
       </c>
       <c r="B31" t="s">
-        <v>94</v>
+        <v>90</v>
+      </c>
+      <c r="C31">
+        <f>3*100*1000</f>
+        <v>300000</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.2">
@@ -942,7 +1057,11 @@
         <v>36</v>
       </c>
       <c r="B33" t="s">
-        <v>93</v>
+        <v>89</v>
+      </c>
+      <c r="C33">
+        <f>21*100*1000</f>
+        <v>2100000</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.2">
@@ -950,7 +1069,11 @@
         <v>37</v>
       </c>
       <c r="B34" t="s">
-        <v>92</v>
+        <v>88</v>
+      </c>
+      <c r="C34">
+        <f>7*100*1000</f>
+        <v>700000</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.2">
@@ -959,6 +1082,10 @@
       </c>
       <c r="B35" t="s">
         <v>85</v>
+      </c>
+      <c r="C35">
+        <f>12*100*1000</f>
+        <v>1200000</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.2">

</xml_diff>